<commit_message>
Changed efficiency to correct value
More details about this change here
</commit_message>
<xml_diff>
--- a/UK.xlsx
+++ b/UK.xlsx
@@ -353,7 +353,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -363,7 +363,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added fuel type to model
</commit_message>
<xml_diff>
--- a/UK.xlsx
+++ b/UK.xlsx
@@ -16,9 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>Oil</t>
   </si>
 </sst>
 </file>
@@ -350,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -366,6 +372,14 @@
         <v>0.9</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added cost to UK
</commit_message>
<xml_diff>
--- a/UK.xlsx
+++ b/UK.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Efficiency</t>
   </si>
@@ -26,12 +26,15 @@
   <si>
     <t>Oil</t>
   </si>
+  <si>
+    <t>Cost</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +71,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -114,7 +125,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -146,9 +157,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -180,6 +192,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -355,16 +368,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -372,11 +385,19 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
     </row>
@@ -386,24 +407,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>